<commit_message>
[feat]create table with sharding support
</commit_message>
<xml_diff>
--- a/jooq-mate-generator/src/test/resources/jooq-mate-config.xlsx
+++ b/jooq-mate-generator/src/test/resources/jooq-mate-config.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27900" windowHeight="13360" activeTab="2"/>
+    <workbookView windowWidth="23100" windowHeight="15060" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="jooq-codegen-config" sheetId="3" r:id="rId1"/>
@@ -401,10 +401,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -424,6 +424,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -445,6 +452,90 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -453,6 +544,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -461,112 +567,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="9"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -599,25 +599,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -629,145 +767,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -792,6 +792,15 @@
       </top>
       <bottom style="thin">
         <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -822,20 +831,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -856,6 +854,21 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -870,26 +883,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -898,148 +898,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="25" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1659,8 +1659,8 @@
   <sheetPr/>
   <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelCol="6"/>

</xml_diff>

<commit_message>
sql generator update table field comment with enums and example
</commit_message>
<xml_diff>
--- a/jooq-mate-generator/src/test/resources/jooq-mate-config.xlsx
+++ b/jooq-mate-generator/src/test/resources/jooq-mate-config.xlsx
@@ -119,7 +119,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="123">
   <si>
     <t>ConfigName</t>
   </si>
@@ -1628,7 +1628,7 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelCol="2"/>
@@ -1750,7 +1750,9 @@
       <c r="B12" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="5"/>
+      <c r="C12" s="5" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="11" t="s">
@@ -1768,7 +1770,9 @@
       <c r="B14" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="5"/>
+      <c r="C14" s="5" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="11" t="s">
@@ -1786,7 +1790,9 @@
       <c r="B16" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="5"/>
+      <c r="C16" s="5" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="11" t="s">

</xml_diff>

<commit_message>
record generator support updatable #9
</commit_message>
<xml_diff>
--- a/jooq-mate-generator/src/test/resources/jooq-mate-config.xlsx
+++ b/jooq-mate-generator/src/test/resources/jooq-mate-config.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="15060" activeTab="1"/>
+    <workbookView windowHeight="15300" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="jooq-codegen-config" sheetId="3" r:id="rId1"/>
@@ -115,6 +115,45 @@
         </r>
       </text>
     </comment>
+    <comment ref="H25" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <rFont val="宋体"/>
+            <charset val="0"/>
+          </rPr>
+          <t>alex:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <rFont val="宋体"/>
+            <charset val="0"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <rFont val="宋体"/>
+            <charset val="0"/>
+          </rPr>
+          <t>will not</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <rFont val="宋体"/>
+            <charset val="0"/>
+          </rPr>
+          <t xml:space="preserve"> generate sql as forign key</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -192,7 +231,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="147">
   <si>
     <t>ConfigName</t>
   </si>
@@ -470,6 +509,15 @@
     <t>example</t>
   </si>
   <si>
+    <t>refKey</t>
+  </si>
+  <si>
+    <t>generateEnum</t>
+  </si>
+  <si>
+    <t>updatable</t>
+  </si>
+  <si>
     <t>主键ID</t>
   </si>
   <si>
@@ -597,12 +645,6 @@
   </si>
   <si>
     <t>parentTableName</t>
-  </si>
-  <si>
-    <t>refKey</t>
-  </si>
-  <si>
-    <t>generateEnum</t>
   </si>
   <si>
     <t>house_layout_test.house_layout_code</t>
@@ -637,10 +679,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -660,13 +702,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -680,6 +715,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -688,11 +731,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -704,8 +746,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="15"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -721,6 +771,14 @@
     </font>
     <font>
       <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
@@ -729,15 +787,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -752,23 +810,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -782,22 +831,15 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -835,13 +877,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -853,25 +1033,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -883,132 +1045,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -1032,21 +1074,16 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -1074,17 +1111,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -1096,6 +1122,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1115,6 +1150,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -1129,157 +1173,168 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="27" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1307,6 +1362,12 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1319,7 +1380,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" quotePrefix="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" quotePrefix="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1662,10 +1723,10 @@
       </c>
     </row>
     <row r="2" ht="17" spans="1:2">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="13" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1743,11 +1804,11 @@
     </row>
   </sheetData>
   <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9:B11">
+      <formula1>"true,false"</formula1>
+    </dataValidation>
     <dataValidation type="textLength" operator="greaterThan" showInputMessage="1" showErrorMessage="1" sqref="B7:B8">
       <formula1>1</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9:B11">
-      <formula1>"true,false"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
       <formula1>"mysql"</formula1>
@@ -1763,7 +1824,7 @@
   <sheetPr/>
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
@@ -1786,10 +1847,10 @@
       </c>
     </row>
     <row r="2" ht="20" customHeight="1" spans="1:3">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="14" t="s">
         <v>20</v>
       </c>
       <c r="C2" s="5" t="s">
@@ -1797,7 +1858,7 @@
       </c>
     </row>
     <row r="3" ht="20" customHeight="1" spans="1:3">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="11" t="s">
         <v>11</v>
       </c>
       <c r="B3" s="8" t="s">
@@ -1806,7 +1867,7 @@
       <c r="C3" s="5"/>
     </row>
     <row r="4" ht="20" customHeight="1" spans="1:3">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="11" t="s">
         <v>22</v>
       </c>
       <c r="B4" s="8" t="s">
@@ -1815,7 +1876,7 @@
       <c r="C4" s="5"/>
     </row>
     <row r="5" ht="20" customHeight="1" spans="1:3">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="11" t="s">
         <v>24</v>
       </c>
       <c r="B5" s="8" t="s">
@@ -1824,7 +1885,7 @@
       <c r="C5" s="5"/>
     </row>
     <row r="6" ht="20" customHeight="1" spans="1:3">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="11" t="s">
         <v>26</v>
       </c>
       <c r="B6" s="8" t="s">
@@ -1833,7 +1894,7 @@
       <c r="C6" s="5"/>
     </row>
     <row r="7" ht="20" customHeight="1" spans="1:3">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="11" t="s">
         <v>13</v>
       </c>
       <c r="B7" s="8" t="s">
@@ -1842,7 +1903,7 @@
       <c r="C7" s="5"/>
     </row>
     <row r="8" ht="20" customHeight="1" spans="1:3">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="11" t="s">
         <v>29</v>
       </c>
       <c r="B8" s="8" t="s">
@@ -1853,7 +1914,7 @@
       </c>
     </row>
     <row r="9" ht="20" customHeight="1" spans="1:3">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="11" t="s">
         <v>31</v>
       </c>
       <c r="B9" s="8"/>
@@ -1862,7 +1923,7 @@
       </c>
     </row>
     <row r="10" ht="20" customHeight="1" spans="1:3">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="11" t="s">
         <v>32</v>
       </c>
       <c r="B10" s="8"/>
@@ -1871,7 +1932,7 @@
       </c>
     </row>
     <row r="11" ht="20" customHeight="1" spans="1:3">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="11" t="s">
         <v>33</v>
       </c>
       <c r="B11" s="8" t="b">
@@ -1880,7 +1941,7 @@
       <c r="C11" s="5"/>
     </row>
     <row r="12" ht="20" customHeight="1" spans="1:3">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="11" t="s">
         <v>34</v>
       </c>
       <c r="B12" s="8" t="b">
@@ -1889,7 +1950,7 @@
       <c r="C12" s="5"/>
     </row>
     <row r="13" ht="20" customHeight="1" spans="1:3">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="11" t="s">
         <v>35</v>
       </c>
       <c r="B13" s="8" t="b">
@@ -1898,7 +1959,7 @@
       <c r="C13" s="5"/>
     </row>
     <row r="14" ht="20" customHeight="1" spans="1:3">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="11" t="s">
         <v>36</v>
       </c>
       <c r="B14" s="8" t="b">
@@ -1907,7 +1968,7 @@
       <c r="C14" s="5"/>
     </row>
     <row r="15" ht="20" customHeight="1" spans="1:3">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="11" t="s">
         <v>37</v>
       </c>
       <c r="B15" s="8"/>
@@ -1974,21 +2035,21 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G36"/>
+  <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
   <cols>
     <col min="1" max="1" width="30.6057692307692" customWidth="1"/>
     <col min="2" max="2" width="39.4134615384615" customWidth="1"/>
     <col min="3" max="3" width="30.6153846153846" customWidth="1"/>
     <col min="4" max="5" width="32.8557692307692" customWidth="1"/>
     <col min="6" max="7" width="35.2596153846154" customWidth="1"/>
-    <col min="8" max="8" width="33.9711538461538" customWidth="1"/>
-    <col min="9" max="9" width="21.4711538461538" customWidth="1"/>
+    <col min="8" max="8" width="29.0096153846154" customWidth="1"/>
+    <col min="9" max="9" width="18.2692307692308" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="35" customHeight="1" spans="1:4">
@@ -2071,7 +2132,7 @@
       <c r="A8" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="14" t="s">
         <v>59</v>
       </c>
       <c r="C8" s="5"/>
@@ -2093,7 +2154,7 @@
       <c r="A10" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="14" t="s">
         <v>63</v>
       </c>
       <c r="C10" s="5"/>
@@ -2237,7 +2298,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="25" s="2" customFormat="1" ht="31" customHeight="1" spans="1:7">
+    <row r="25" s="2" customFormat="1" ht="31" customHeight="1" spans="1:10">
       <c r="A25" s="7" t="s">
         <v>86</v>
       </c>
@@ -2259,199 +2320,261 @@
       <c r="G25" s="7" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="26" ht="20" customHeight="1" spans="1:7">
-      <c r="A26" t="s">
+      <c r="H25" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="I25" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="J25" s="10" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="26" ht="20" customHeight="1" spans="1:10">
+      <c r="A26" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="B26" t="s">
-        <v>92</v>
-      </c>
-      <c r="C26" t="s">
-        <v>93</v>
-      </c>
+      <c r="B26" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
       <c r="G26" s="8" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="27" ht="20" customHeight="1" spans="1:7">
-      <c r="A27" t="s">
+        <v>97</v>
+      </c>
+      <c r="H26" s="9"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="9"/>
+    </row>
+    <row r="27" ht="20" customHeight="1" spans="1:10">
+      <c r="A27" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="B27" t="s">
-        <v>95</v>
-      </c>
-      <c r="C27" t="s">
+      <c r="B27" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="D27" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="G27" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="H27" s="9"/>
+      <c r="I27" s="9"/>
+      <c r="J27" s="9"/>
+    </row>
+    <row r="28" ht="20" customHeight="1" spans="1:10">
+      <c r="A28" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="D28" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="H28" s="9"/>
+      <c r="I28" s="9"/>
+      <c r="J28" s="9"/>
+    </row>
+    <row r="29" ht="20" customHeight="1" spans="1:10">
+      <c r="A29" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="D29" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="E29" s="9"/>
+      <c r="F29" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="G29" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="H29" s="9"/>
+      <c r="I29" s="9"/>
+      <c r="J29" s="9"/>
+    </row>
+    <row r="30" ht="20" customHeight="1" spans="1:10">
+      <c r="A30" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="D30" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="E30" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="F30" s="9"/>
+      <c r="G30" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="H30" s="9"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="9"/>
+    </row>
+    <row r="31" ht="20" customHeight="1" spans="1:10">
+      <c r="A31" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="D31" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="H31" s="9"/>
+      <c r="I31" s="9"/>
+      <c r="J31" s="9"/>
+    </row>
+    <row r="32" ht="20" customHeight="1" spans="1:10">
+      <c r="A32" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="C32" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="D27" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="F27" t="s">
-        <v>98</v>
-      </c>
-      <c r="G27" s="8" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="28" ht="20" customHeight="1" spans="1:7">
-      <c r="A28" t="s">
+      <c r="D32" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="H32" s="9"/>
+      <c r="I32" s="9"/>
+      <c r="J32" s="9"/>
+    </row>
+    <row r="33" ht="20" customHeight="1" spans="1:10">
+      <c r="A33" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="D33" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="B28" t="s">
-        <v>101</v>
-      </c>
-      <c r="C28" t="s">
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="D28" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="G28" s="8" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="29" ht="20" customHeight="1" spans="1:7">
-      <c r="A29" t="s">
-        <v>104</v>
-      </c>
-      <c r="B29" t="s">
-        <v>105</v>
-      </c>
-      <c r="C29" t="s">
+      <c r="H33" s="9"/>
+      <c r="I33" s="9"/>
+      <c r="J33" s="9"/>
+    </row>
+    <row r="34" ht="20" customHeight="1" spans="1:10">
+      <c r="A34" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="D34" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="D29" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="F29" s="13" t="s">
-        <v>108</v>
-      </c>
-      <c r="G29" s="8" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="30" ht="20" customHeight="1" spans="1:7">
-      <c r="A30" t="s">
-        <v>109</v>
-      </c>
-      <c r="B30" t="s">
-        <v>110</v>
-      </c>
-      <c r="C30" t="s">
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="D30" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="E30" t="s">
-        <v>112</v>
-      </c>
-      <c r="G30" s="8" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="31" ht="20" customHeight="1" spans="1:7">
-      <c r="A31" t="s">
-        <v>113</v>
-      </c>
-      <c r="B31" t="s">
-        <v>114</v>
-      </c>
-      <c r="C31" t="s">
-        <v>115</v>
-      </c>
-      <c r="D31" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="G31" s="8" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="32" ht="20" customHeight="1" spans="1:7">
-      <c r="A32" t="s">
-        <v>116</v>
-      </c>
-      <c r="B32" t="s">
-        <v>117</v>
-      </c>
-      <c r="C32" t="s">
-        <v>93</v>
-      </c>
-      <c r="D32" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="G32" s="8" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="33" ht="20" customHeight="1" spans="1:7">
-      <c r="A33" t="s">
-        <v>118</v>
-      </c>
-      <c r="B33" t="s">
-        <v>119</v>
-      </c>
-      <c r="C33" t="s">
-        <v>115</v>
-      </c>
-      <c r="D33" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="G33" s="8" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="34" ht="20" customHeight="1" spans="1:7">
-      <c r="A34" t="s">
-        <v>120</v>
-      </c>
-      <c r="B34" t="s">
-        <v>121</v>
-      </c>
-      <c r="C34" t="s">
-        <v>93</v>
-      </c>
-      <c r="D34" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="G34" s="8" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="35" ht="20" customHeight="1" spans="1:7">
-      <c r="A35" t="s">
-        <v>122</v>
-      </c>
-      <c r="B35" t="s">
-        <v>123</v>
-      </c>
-      <c r="C35" t="s">
-        <v>124</v>
-      </c>
-      <c r="D35" t="s">
+      <c r="H34" s="9"/>
+      <c r="I34" s="9"/>
+      <c r="J34" s="9"/>
+    </row>
+    <row r="35" ht="20" customHeight="1" spans="1:10">
+      <c r="A35" s="9" t="s">
         <v>125</v>
       </c>
+      <c r="B35" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
       <c r="G35" s="8" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="36" ht="20" customHeight="1" spans="1:7">
-      <c r="A36" t="s">
-        <v>126</v>
-      </c>
-      <c r="B36" t="s">
+        <v>102</v>
+      </c>
+      <c r="H35" s="9"/>
+      <c r="I35" s="9"/>
+      <c r="J35" s="9"/>
+    </row>
+    <row r="36" ht="20" customHeight="1" spans="1:10">
+      <c r="A36" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="C36" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="C36" t="s">
-        <v>124</v>
-      </c>
-      <c r="D36" t="s">
-        <v>125</v>
-      </c>
+      <c r="D36" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="E36" s="9"/>
+      <c r="F36" s="9"/>
       <c r="G36" s="8" t="s">
-        <v>99</v>
-      </c>
+        <v>102</v>
+      </c>
+      <c r="H36" s="9"/>
+      <c r="I36" s="9"/>
+      <c r="J36" s="9"/>
     </row>
   </sheetData>
   <dataValidations count="2">
@@ -2471,10 +2594,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I36"/>
+  <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -2507,7 +2630,7 @@
         <v>45</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
@@ -2517,7 +2640,7 @@
         <v>47</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
@@ -2527,7 +2650,7 @@
         <v>49</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -2537,7 +2660,7 @@
         <v>51</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
@@ -2550,7 +2673,7 @@
         <v>54</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="D6" s="5"/>
     </row>
@@ -2568,8 +2691,8 @@
       <c r="A8" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B8" s="12" t="s">
-        <v>133</v>
+      <c r="B8" s="14" t="s">
+        <v>136</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5" t="s">
@@ -2590,7 +2713,7 @@
       <c r="A10" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="14" t="s">
         <v>63</v>
       </c>
       <c r="C10" s="5"/>
@@ -2598,7 +2721,7 @@
     </row>
     <row r="11" ht="20" customHeight="1" spans="1:4">
       <c r="A11" s="4" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>46</v>
@@ -2655,7 +2778,7 @@
         <v>73</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="5" t="s">
@@ -2724,7 +2847,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="25" s="2" customFormat="1" ht="31" customHeight="1" spans="1:9">
+    <row r="25" s="2" customFormat="1" ht="31" customHeight="1" spans="1:10">
       <c r="A25" s="7" t="s">
         <v>86</v>
       </c>
@@ -2747,248 +2870,262 @@
         <v>58</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>135</v>
+        <v>92</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="26" ht="20" customHeight="1" spans="1:9">
+        <v>93</v>
+      </c>
+      <c r="J25" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="26" ht="20" customHeight="1" spans="1:10">
       <c r="A26" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
       <c r="G26" s="8" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="H26" s="5"/>
       <c r="I26" s="5"/>
-    </row>
-    <row r="27" ht="20" customHeight="1" spans="1:9">
+      <c r="J26" s="9"/>
+    </row>
+    <row r="27" ht="20" customHeight="1" spans="1:10">
       <c r="A27" t="s">
         <v>55</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="D27" s="12" t="s">
-        <v>97</v>
+        <v>99</v>
+      </c>
+      <c r="D27" s="14" t="s">
+        <v>100</v>
       </c>
       <c r="E27" s="5"/>
       <c r="F27" s="5" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="G27" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="H27" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="I27" s="5"/>
+      <c r="J27" s="9"/>
+    </row>
+    <row r="28" ht="20" customHeight="1" spans="1:10">
+      <c r="A28" t="s">
+        <v>139</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="C28" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="H27" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="I27" s="5"/>
-    </row>
-    <row r="28" ht="20" customHeight="1" spans="1:9">
-      <c r="A28" t="s">
-        <v>138</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="D28" s="12" t="s">
-        <v>97</v>
+      <c r="D28" s="14" t="s">
+        <v>100</v>
       </c>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
       <c r="G28" s="8" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="H28" s="5"/>
       <c r="I28" s="5"/>
-    </row>
-    <row r="29" ht="20" customHeight="1" spans="1:9">
+      <c r="J28" s="9"/>
+    </row>
+    <row r="29" ht="20" customHeight="1" spans="1:10">
       <c r="A29" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="D29" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="D29" s="14" t="s">
         <v>63</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="F29" s="5"/>
       <c r="G29" s="8" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="H29" s="5"/>
       <c r="I29" s="5"/>
-    </row>
-    <row r="30" ht="20" customHeight="1" spans="1:9">
+      <c r="J29" s="9"/>
+    </row>
+    <row r="30" ht="20" customHeight="1" spans="1:10">
       <c r="A30" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="D30" s="12" t="s">
-        <v>111</v>
+        <v>105</v>
+      </c>
+      <c r="D30" s="14" t="s">
+        <v>114</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F30" s="5"/>
       <c r="G30" s="8" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="H30" s="5"/>
       <c r="I30" s="5"/>
-    </row>
-    <row r="31" ht="20" customHeight="1" spans="1:9">
+      <c r="J30" s="9"/>
+    </row>
+    <row r="31" ht="20" customHeight="1" spans="1:10">
       <c r="A31" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="D31" s="12" t="s">
-        <v>97</v>
+        <v>118</v>
+      </c>
+      <c r="D31" s="14" t="s">
+        <v>100</v>
       </c>
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
       <c r="G31" s="8" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="H31" s="5"/>
       <c r="I31" s="5"/>
-    </row>
-    <row r="32" ht="20" customHeight="1" spans="1:9">
+      <c r="J31" s="9"/>
+    </row>
+    <row r="32" ht="20" customHeight="1" spans="1:10">
       <c r="A32" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="D32" s="12" t="s">
-        <v>103</v>
+        <v>96</v>
+      </c>
+      <c r="D32" s="14" t="s">
+        <v>106</v>
       </c>
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
       <c r="G32" s="8" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="H32" s="5"/>
       <c r="I32" s="5"/>
-    </row>
-    <row r="33" ht="20" customHeight="1" spans="1:9">
+      <c r="J32" s="9"/>
+    </row>
+    <row r="33" ht="20" customHeight="1" spans="1:10">
       <c r="A33" t="s">
+        <v>121</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C33" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="B33" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="D33" s="12" t="s">
-        <v>97</v>
+      <c r="D33" s="14" t="s">
+        <v>100</v>
       </c>
       <c r="E33" s="5"/>
       <c r="F33" s="5"/>
       <c r="G33" s="8" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="H33" s="5"/>
       <c r="I33" s="5"/>
-    </row>
-    <row r="34" ht="20" customHeight="1" spans="1:9">
+      <c r="J33" s="9"/>
+    </row>
+    <row r="34" ht="20" customHeight="1" spans="1:10">
       <c r="A34" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="D34" s="12" t="s">
-        <v>103</v>
+        <v>96</v>
+      </c>
+      <c r="D34" s="14" t="s">
+        <v>106</v>
       </c>
       <c r="E34" s="5"/>
       <c r="F34" s="5"/>
       <c r="G34" s="8" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="H34" s="5"/>
       <c r="I34" s="5"/>
-    </row>
-    <row r="35" ht="20" customHeight="1" spans="1:9">
+      <c r="J34" s="9"/>
+    </row>
+    <row r="35" ht="20" customHeight="1" spans="1:10">
       <c r="A35" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="E35" s="5"/>
       <c r="F35" s="5"/>
       <c r="G35" s="8" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="H35" s="5"/>
       <c r="I35" s="5"/>
-    </row>
-    <row r="36" ht="20" customHeight="1" spans="1:9">
+      <c r="J35" s="9"/>
+    </row>
+    <row r="36" ht="20" customHeight="1" spans="1:10">
       <c r="A36" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="B36" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="C36" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="C36" s="5" t="s">
-        <v>124</v>
-      </c>
       <c r="D36" s="5" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="E36" s="5"/>
       <c r="F36" s="5"/>
       <c r="G36" s="8" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="H36" s="5"/>
       <c r="I36" s="5"/>
+      <c r="J36" s="9"/>
     </row>
   </sheetData>
   <dataValidations count="2">
@@ -3007,6 +3144,9 @@
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="https://web.wps.cn/et/2018/main" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <commentList sheetStid="1">
+    <comment s:ref="H25" rgbClr="896C9C"/>
+  </commentList>
   <commentList sheetStid="4">
     <comment s:ref="E25" rgbClr="896C9C"/>
     <comment s:ref="H25" rgbClr="896C9C"/>

</xml_diff>